<commit_message>
added the 2nd reset pin to enable the FTDI programming
</commit_message>
<xml_diff>
--- a/docs/satshakit_128.xlsx
+++ b/docs/satshakit_128.xlsx
@@ -147,7 +147,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -182,6 +182,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -190,17 +191,12 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u val="single"/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -262,15 +258,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -298,21 +294,21 @@
   <dimension ref="A1:J65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -557,10 +553,10 @@
         <v>0.0354</v>
       </c>
       <c r="G9" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9" s="6" t="n">
-        <v>0.35</v>
+        <v>0.7</v>
       </c>
       <c r="J9" s="3"/>
     </row>
@@ -724,7 +720,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="7" t="n">
         <f aca="false">SUM(H3:H15)</f>
-        <v>13.188</v>
+        <v>13.538</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>